<commit_message>
changed type name from open-num and open-char to numeric and string
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects and porfolio\Projects\self\R Shiny Survey Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD9A904-81CD-4AB1-AAFB-4821733096C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{416847CC-37DE-4297-BC2E-62AD6A21C215}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,9 +54,6 @@
     <t>How old are you?</t>
   </si>
   <si>
-    <t>open-num</t>
-  </si>
-  <si>
     <t>Personal Info</t>
   </si>
   <si>
@@ -72,9 +69,6 @@
     <t>What is your favourate R package?</t>
   </si>
   <si>
-    <t>open-char</t>
-  </si>
-  <si>
     <t>date</t>
   </si>
   <si>
@@ -103,6 +97,12 @@
   </si>
   <si>
     <t>1,100,20</t>
+  </si>
+  <si>
+    <t>numeric</t>
+  </si>
+  <si>
+    <t>string</t>
   </si>
 </sst>
 </file>
@@ -423,7 +423,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,91 +470,92 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
         <v>20</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
         <v>17</v>
       </c>
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" t="s">
-        <v>19</v>
-      </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
data store and see results
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects and porfolio\Projects\self\R Shiny Survey Tool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Projects and porfolio\Projects\self\R Shiny Survey Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{416847CC-37DE-4297-BC2E-62AD6A21C215}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E4AB6D-CFD4-4034-9AA3-CADE710FBDAE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>Module</t>
   </si>
@@ -73,12 +73,6 @@
   </si>
   <si>
     <t>Others</t>
-  </si>
-  <si>
-    <t>Pick a date range</t>
-  </si>
-  <si>
-    <t>date-range</t>
   </si>
   <si>
     <t>Pick a date</t>
@@ -420,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,10 +464,10 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -484,10 +478,10 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -512,7 +506,7 @@
         <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -520,13 +514,13 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
         <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -534,24 +528,10 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
         <v>17</v>
-      </c>
-      <c r="D8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed previous submission table update issue
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Projects and porfolio\Projects\self\R Shiny Survey Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E4AB6D-CFD4-4034-9AA3-CADE710FBDAE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F40CD264-DFEE-4873-984C-18AC1660C79D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3465" yWindow="960" windowWidth="21075" windowHeight="12525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="questions" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t>Module</t>
   </si>
@@ -84,9 +84,6 @@
     <t>2020-01-01,2020-12-31</t>
   </si>
   <si>
-    <t>Pick a time (24 hrs)</t>
-  </si>
-  <si>
     <t>1,27,3</t>
   </si>
   <si>
@@ -97,6 +94,12 @@
   </si>
   <si>
     <t>string</t>
+  </si>
+  <si>
+    <t>Pick a time</t>
+  </si>
+  <si>
+    <t>09:00,17:00,12:00</t>
   </si>
 </sst>
 </file>
@@ -417,7 +420,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,10 +467,10 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -478,10 +481,10 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -506,7 +509,7 @@
         <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -528,10 +531,13 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
         <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>